<commit_message>
Added some guesstimate hours
</commit_message>
<xml_diff>
--- a/TimeManager.xlsx
+++ b/TimeManager.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/917b0c1e9539ad85/Spring17/CSC131/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew's PC\Documents\GitHub\No-Preference-CSC-131\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -412,7 +412,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,6 +488,12 @@
       <c r="A3" s="1">
         <v>42806</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
       <c r="M3">
         <f>SUM(D3+F3+H3+J3)</f>
         <v>0</v>
@@ -558,11 +564,11 @@
       </c>
       <c r="B9">
         <f>SUM(B3:B7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f>SUM(C3:C7)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <f t="shared" ref="D9:K9" si="2">SUM(D3:D7)</f>

</xml_diff>